<commit_message>
Replace use of escape() with encodeURIComponent(). Changes to launch a form from an external link construction. Changes to support values_list filtering on instances prompt.
</commit_message>
<xml_diff>
--- a/app/tables/Ethiopia_household/forms/Ethiopia_household_data/Ethiopia_household_data.xlsx
+++ b/app/tables/Ethiopia_household/forms/Ethiopia_household_data/Ethiopia_household_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="0" windowWidth="25540" windowHeight="16060" tabRatio="500"/>
@@ -124,9 +124,6 @@
     <t>Ethiopia Household Data</t>
   </si>
   <si>
-    <t>'household_id='+escape(data('household_id'))</t>
-  </si>
-  <si>
     <t>primary_languages</t>
   </si>
   <si>
@@ -989,6 +986,9 @@
   </si>
   <si>
     <t>filters by both the household_id and the age</t>
+  </si>
+  <si>
+    <t>'household_id='+encodeURIComponent(data('household_id'))</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1295,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1421,9 +1421,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1600,6 +1597,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1927,11 +1929,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
@@ -1943,21 +1945,21 @@
     <col min="8" max="8" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="46" customFormat="1">
+    <row r="1" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="44" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="44" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>22</v>
@@ -1969,9 +1971,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="2" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
@@ -1981,9 +1983,9 @@
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
     </row>
-    <row r="3" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="3" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="36" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
@@ -1993,9 +1995,9 @@
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
     </row>
-    <row r="4" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="4" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
@@ -2005,9 +2007,9 @@
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
     </row>
-    <row r="5" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="5" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="36" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
@@ -2017,9 +2019,9 @@
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
     </row>
-    <row r="6" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="6" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -2029,9 +2031,9 @@
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
     </row>
-    <row r="7" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="7" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
@@ -2041,7 +2043,7 @@
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
     </row>
-    <row r="8" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
+    <row r="8" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36"/>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -2051,18 +2053,18 @@
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
     </row>
-    <row r="9" spans="1:17" ht="45">
+    <row r="9" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>28</v>
@@ -2074,43 +2076,43 @@
         <v>25</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>28</v>
@@ -2122,33 +2124,33 @@
         <v>25</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="12" customFormat="1" ht="30" customHeight="1">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="12" t="s">
         <v>28</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="H12" s="49" t="s">
-        <v>31</v>
+        <v>54</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>319</v>
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -2156,15 +2158,15 @@
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
     </row>
-    <row r="13" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="13" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>28</v>
@@ -2176,7 +2178,7 @@
         <v>25</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -2184,15 +2186,15 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>28</v>
@@ -2201,10 +2203,10 @@
         <v>23</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -2212,27 +2214,27 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
@@ -2240,27 +2242,27 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
     </row>
-    <row r="16" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="16" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -2268,27 +2270,27 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="17" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -2296,27 +2298,27 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
     </row>
-    <row r="18" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="18" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -2324,27 +2326,27 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="19" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
@@ -2352,15 +2354,15 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="20" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>28</v>
@@ -2372,7 +2374,7 @@
         <v>25</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -2380,15 +2382,15 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="21" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>28</v>
@@ -2400,7 +2402,7 @@
         <v>25</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -2408,16 +2410,16 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>28</v>
@@ -2426,22 +2428,22 @@
         <v>23</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>28</v>
@@ -2453,19 +2455,19 @@
         <v>25</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>28</v>
@@ -2477,19 +2479,19 @@
         <v>25</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>28</v>
@@ -2501,7 +2503,7 @@
         <v>25</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -2523,7 +2525,7 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
@@ -2538,21 +2540,21 @@
     <col min="11" max="11" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="45" customFormat="1" ht="30">
+    <row r="1" spans="1:15" s="45" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>19</v>
@@ -2564,26 +2566,26 @@
         <v>7</v>
       </c>
       <c r="I1" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J1" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K1" s="44" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
       <c r="N1" s="44"/>
       <c r="O1" s="44"/>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1">
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -2591,19 +2593,19 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="90">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="93" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>212</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -2611,13 +2613,13 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" s="10" customFormat="1" ht="30">
+    <row r="4" spans="1:15" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -2625,19 +2627,19 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:15" s="10" customFormat="1" ht="30">
+    <row r="5" spans="1:15" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
       <c r="D5" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -2645,35 +2647,35 @@
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
     </row>
-    <row r="6" spans="1:15" s="10" customFormat="1" ht="75">
+    <row r="6" spans="1:15" s="10" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
       <c r="D6" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="I6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>219</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:15" s="10" customFormat="1">
+    <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -2681,19 +2683,19 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="1:15" s="10" customFormat="1" ht="30">
+    <row r="8" spans="1:15" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
       <c r="D8" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E8" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>222</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>223</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -2701,10 +2703,10 @@
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
     </row>
-    <row r="9" spans="1:15" s="10" customFormat="1">
+    <row r="9" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -2712,19 +2714,19 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="45">
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -2732,13 +2734,13 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" s="12" customFormat="1" ht="30">
+    <row r="11" spans="1:15" s="12" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
@@ -2746,19 +2748,19 @@
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
     </row>
-    <row r="12" spans="1:15" s="12" customFormat="1" ht="30">
+    <row r="12" spans="1:15" s="12" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
       <c r="D12" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F12" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>243</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>244</v>
       </c>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
@@ -2766,35 +2768,35 @@
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
     </row>
-    <row r="13" spans="1:15" s="12" customFormat="1" ht="75">
+    <row r="13" spans="1:15" s="12" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
       <c r="D13" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="I13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" s="11" t="s">
         <v>246</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>247</v>
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
     </row>
-    <row r="14" spans="1:15" s="12" customFormat="1">
+    <row r="14" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11"/>
       <c r="B14" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
@@ -2802,7 +2804,7 @@
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
     </row>
-    <row r="15" spans="1:15" s="28" customFormat="1">
+    <row r="15" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="27"/>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
@@ -2810,13 +2812,13 @@
       <c r="N15" s="27"/>
       <c r="O15" s="27"/>
     </row>
-    <row r="16" spans="1:15" s="1" customFormat="1">
+    <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="D16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -2824,19 +2826,19 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" ht="60">
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="62" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="D17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>251</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -2844,13 +2846,13 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:15" s="26" customFormat="1" ht="30">
+    <row r="18" spans="1:15" s="26" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="16"/>
       <c r="B18" s="26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
@@ -2858,19 +2860,19 @@
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
     </row>
-    <row r="19" spans="1:15" s="26" customFormat="1" ht="30">
+    <row r="19" spans="1:15" s="26" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="16"/>
       <c r="D19" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="G19" s="26" t="s">
         <v>254</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="G19" s="26" t="s">
-        <v>255</v>
       </c>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
@@ -2878,19 +2880,19 @@
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
     </row>
-    <row r="20" spans="1:15" s="26" customFormat="1" ht="30">
+    <row r="20" spans="1:15" s="26" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A20" s="16"/>
       <c r="D20" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="G20" s="26" t="s">
         <v>257</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>258</v>
       </c>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
@@ -2898,13 +2900,13 @@
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
     </row>
-    <row r="21" spans="1:15" s="10" customFormat="1" ht="30">
+    <row r="21" spans="1:15" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
       <c r="B21" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
@@ -2912,19 +2914,19 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
     </row>
-    <row r="22" spans="1:15" s="10" customFormat="1">
+    <row r="22" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="D22" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>272</v>
-      </c>
       <c r="G22" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
@@ -2932,13 +2934,13 @@
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="1:15" s="8" customFormat="1" ht="30">
+    <row r="23" spans="1:15" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
       <c r="B23" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
@@ -2946,16 +2948,16 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="1:15" s="8" customFormat="1">
+    <row r="24" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
       <c r="D24" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>282</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>283</v>
       </c>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
@@ -2963,10 +2965,10 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="1:15" s="8" customFormat="1">
+    <row r="25" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
       <c r="B25" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
@@ -2974,10 +2976,10 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="1:15" s="10" customFormat="1">
+    <row r="26" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
@@ -2985,10 +2987,10 @@
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
     </row>
-    <row r="27" spans="1:15" s="26" customFormat="1">
+    <row r="27" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16"/>
       <c r="B27" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K27" s="16"/>
       <c r="L27" s="16"/>
@@ -2996,7 +2998,7 @@
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
     </row>
-    <row r="28" spans="1:15" s="1" customFormat="1">
+    <row r="28" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -3004,32 +3006,32 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="1:15" s="1" customFormat="1">
+    <row r="29" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="D29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:15" s="1" customFormat="1" ht="60">
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="62" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="D30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
@@ -3037,13 +3039,13 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" spans="1:15" s="12" customFormat="1" ht="30">
+    <row r="31" spans="1:15" s="12" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="11"/>
       <c r="B31" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
@@ -3051,28 +3053,28 @@
       <c r="N31" s="11"/>
       <c r="O31" s="11"/>
     </row>
-    <row r="32" spans="1:15" s="12" customFormat="1">
+    <row r="32" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11"/>
       <c r="D32" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I32" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J32" s="12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" s="12" customFormat="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11"/>
       <c r="B33" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
@@ -3080,36 +3082,36 @@
       <c r="N33" s="11"/>
       <c r="O33" s="11"/>
     </row>
-    <row r="34" spans="1:15" s="30" customFormat="1" ht="45">
+    <row r="34" spans="1:15" s="30" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A34" s="29" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>1</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G34" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="H34" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="H34" s="30" t="s">
-        <v>62</v>
-      </c>
       <c r="I34" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J34" s="30" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" s="1" customFormat="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="D35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
@@ -3117,15 +3119,15 @@
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E36" t="s">
+        <v>293</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>294</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>
@@ -3134,23 +3136,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D38" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I38" t="b">
         <v>1</v>
@@ -3178,7 +3180,7 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="3" max="3" width="33.83203125" customWidth="1"/>
@@ -3189,21 +3191,21 @@
     <col min="8" max="8" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
+    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>19</v>
@@ -3220,16 +3222,16 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="105">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -3237,21 +3239,21 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -3259,12 +3261,12 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="32" customFormat="1" ht="45">
+    <row r="4" spans="1:13" s="32" customFormat="1" ht="62" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -3277,9 +3279,9 @@
       <c r="L4" s="31"/>
       <c r="M4" s="31"/>
     </row>
-    <row r="5" spans="1:13" s="32" customFormat="1" ht="30">
+    <row r="5" spans="1:13" s="32" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
@@ -3288,10 +3290,10 @@
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I5" s="31"/>
       <c r="J5" s="31"/>
@@ -3299,13 +3301,13 @@
       <c r="L5" s="31"/>
       <c r="M5" s="31"/>
     </row>
-    <row r="6" spans="1:13" s="10" customFormat="1" ht="30">
+    <row r="6" spans="1:13" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -3317,21 +3319,21 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" s="10" customFormat="1">
+    <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -3339,10 +3341,10 @@
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1">
+    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -3355,10 +3357,10 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" s="32" customFormat="1">
+    <row r="9" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="31"/>
       <c r="B9" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
@@ -3371,21 +3373,21 @@
       <c r="L9" s="31"/>
       <c r="M9" s="31"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -3393,10 +3395,10 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" s="25" customFormat="1" ht="30">
+    <row r="11" spans="1:13" s="25" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="17"/>
       <c r="B11" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -3409,21 +3411,21 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
     </row>
-    <row r="12" spans="1:13" s="25" customFormat="1" ht="30">
+    <row r="12" spans="1:13" s="25" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
@@ -3431,13 +3433,13 @@
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
     </row>
-    <row r="13" spans="1:13" s="10" customFormat="1">
+    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -3449,21 +3451,21 @@
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" s="10" customFormat="1" ht="30">
+    <row r="14" spans="1:13" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E14" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -3471,10 +3473,10 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" s="10" customFormat="1">
+    <row r="15" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -3487,10 +3489,10 @@
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" s="25" customFormat="1">
+    <row r="16" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17"/>
       <c r="B16" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -3503,21 +3505,21 @@
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
     </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="17" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -3525,13 +3527,13 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" s="12" customFormat="1" ht="30">
+    <row r="18" spans="1:13" s="12" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
@@ -3543,9 +3545,9 @@
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
     </row>
-    <row r="19" spans="1:13" s="12" customFormat="1" ht="30">
+    <row r="19" spans="1:13" s="12" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -3554,10 +3556,10 @@
       </c>
       <c r="E19" s="11"/>
       <c r="F19" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -3565,10 +3567,10 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" s="12" customFormat="1">
+    <row r="20" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -3581,21 +3583,21 @@
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
     </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -3603,21 +3605,21 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="22" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -3644,7 +3646,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
@@ -3656,21 +3658,21 @@
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
+    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>19</v>
@@ -3687,9 +3689,9 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" ht="45">
+    <row r="2" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>18</v>
@@ -3701,12 +3703,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="5" spans="1:13" s="6" customFormat="1" ht="62" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -3714,10 +3716,10 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="7" spans="1:13" s="6" customFormat="1">
+    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -3725,10 +3727,10 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1">
+    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -3736,10 +3738,10 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
     </row>
-    <row r="11" spans="1:13" s="6" customFormat="1">
+    <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -3747,10 +3749,10 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
     </row>
-    <row r="13" spans="1:13" s="6" customFormat="1">
+    <row r="13" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -3758,10 +3760,10 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="15" spans="1:13" s="6" customFormat="1">
+    <row r="15" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -3769,10 +3771,10 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="17" spans="1:13" s="6" customFormat="1">
+    <row r="17" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -3799,275 +3801,275 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="46" customFormat="1">
+    <row r="1" spans="1:3" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>68</v>
       </c>
       <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="37" customFormat="1">
+    <row r="2" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" s="37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="37" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="37" customFormat="1">
-      <c r="A3" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>115</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="38" customFormat="1">
+    <row r="4" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="16" t="s">
+    </row>
+    <row r="5" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="38" customFormat="1">
-      <c r="A5" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="16" t="s">
+    </row>
+    <row r="6" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" s="39" customFormat="1">
-      <c r="A6" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" s="39" customFormat="1">
-      <c r="A7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="7" t="s">
+    </row>
+    <row r="8" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" s="39" customFormat="1">
-      <c r="A8" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="40" customFormat="1">
+    </row>
+    <row r="9" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="40" customFormat="1">
-      <c r="A10" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B10" s="9" t="s">
+    <row r="11" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="40" customFormat="1">
-      <c r="A11" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B11" s="9" t="s">
+    <row r="12" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="40" customFormat="1">
-      <c r="A12" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B12" s="9" t="s">
+    <row r="13" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="40" customFormat="1">
-      <c r="A13" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B13" s="9" t="s">
+    <row r="14" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="40" customFormat="1">
-      <c r="A14" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B14" s="9" t="s">
+    <row r="15" spans="1:3" s="40" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="40" customFormat="1" ht="30">
-      <c r="A15" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="41" customFormat="1">
+    <row r="16" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="41" customFormat="1">
-      <c r="A17" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="C17" s="11" t="s">
+    <row r="18" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" s="42" customFormat="1">
-      <c r="A18" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="B18" s="13" t="s">
+      <c r="C18" s="13" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C19" s="13" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="42" customFormat="1">
-      <c r="A19" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="B19" s="13" t="s">
+    <row r="20" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C20" s="13" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="42" customFormat="1">
-      <c r="A20" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="43" customFormat="1">
+    <row r="21" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B21" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C22" s="17" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="43" customFormat="1">
-      <c r="A22" s="17" t="s">
-        <v>271</v>
-      </c>
-      <c r="B22" s="17" t="s">
+    <row r="23" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C23" s="17" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="43" customFormat="1">
-      <c r="A23" s="17" t="s">
-        <v>271</v>
-      </c>
-      <c r="B23" s="17" t="s">
+    <row r="24" spans="1:3" s="43" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A24" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C24" s="17" t="s">
         <v>279</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="43" customFormat="1" ht="30">
-      <c r="A24" s="17" t="s">
-        <v>271</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>276</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -4089,7 +4091,7 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" style="3" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="3" customWidth="1"/>
@@ -4098,7 +4100,7 @@
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="44" customFormat="1">
+    <row r="1" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>11</v>
       </c>
@@ -4109,10 +4111,10 @@
         <v>13</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -4121,7 +4123,7 @@
       </c>
       <c r="D2" s="48"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -4130,7 +4132,7 @@
       </c>
       <c r="D3" s="48"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -4139,7 +4141,7 @@
       </c>
       <c r="D4" s="48"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -4148,74 +4150,74 @@
       </c>
       <c r="D5" s="48"/>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D6" s="48" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="48"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D7" s="48"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
+      <c r="D8" s="48"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D8" s="48"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="48"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D9" s="48"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="48"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D10" s="48"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="48"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D11" s="48"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="D12" s="48"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>20</v>
@@ -4241,7 +4243,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="39.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="3" customWidth="1"/>
@@ -4254,15 +4256,15 @@
     <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1">
+    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>2</v>
@@ -4271,13 +4273,13 @@
         <v>7</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -4285,7 +4287,7 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="33" customHeight="1">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -4301,15 +4303,15 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="76" customHeight="1">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -4318,7 +4320,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -4326,24 +4328,24 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" ht="109" customHeight="1">
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="109" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -4370,7 +4372,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
     <col min="2" max="2" width="12.5" style="3" customWidth="1"/>
@@ -4381,33 +4383,33 @@
     <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="44" customFormat="1">
+    <row r="1" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" s="44" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="3"/>
@@ -4416,29 +4418,29 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1">
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1">
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="C4" s="3"/>
       <c r="G4" s="3"/>
@@ -4465,7 +4467,7 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
@@ -4476,15 +4478,15 @@
     <col min="7" max="7" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="46" customFormat="1">
+    <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" s="44" t="s">
         <v>19</v>
@@ -4493,23 +4495,23 @@
         <v>2</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
       <c r="K1" s="44"/>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -4517,151 +4519,151 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="30">
+    <row r="3" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="90">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="93" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="45">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="45">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" ht="30">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" ht="30">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" ht="45">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" ht="45">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" ht="30">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -4674,7 +4676,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -4687,7 +4689,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -4700,7 +4702,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -4713,7 +4715,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -4726,7 +4728,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -4739,7 +4741,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4752,7 +4754,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -4765,7 +4767,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -4778,7 +4780,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -4791,7 +4793,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4804,7 +4806,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4817,7 +4819,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4830,7 +4832,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4862,7 +4864,7 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="37.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" style="3" customWidth="1"/>
@@ -4877,21 +4879,21 @@
     <col min="11" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" ht="30">
+    <row r="1" spans="1:13" s="45" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>19</v>
@@ -4900,25 +4902,25 @@
         <v>2</v>
       </c>
       <c r="H1" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K1" s="44"/>
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -4926,32 +4928,32 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="30">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="8" customFormat="1">
+    <row r="4" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -4962,21 +4964,21 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" s="8" customFormat="1">
+    <row r="5" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>125</v>
-      </c>
       <c r="G5" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -4985,10 +4987,10 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" s="8" customFormat="1">
+    <row r="6" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -5001,19 +5003,19 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" s="8" customFormat="1" ht="60">
+    <row r="7" spans="1:13" s="8" customFormat="1" ht="62" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="D7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -5022,13 +5024,13 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1">
+    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -5041,19 +5043,19 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" s="10" customFormat="1">
+    <row r="9" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="D9" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F9" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>130</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>131</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -5062,10 +5064,10 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" s="10" customFormat="1">
+    <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -5078,10 +5080,10 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" s="8" customFormat="1">
+    <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -5094,13 +5096,13 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13" s="14" customFormat="1">
+    <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13"/>
       <c r="B12" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
@@ -5109,36 +5111,36 @@
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="1:13" s="14" customFormat="1" ht="90">
+    <row r="13" spans="1:13" s="14" customFormat="1" ht="93" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
-    <row r="14" spans="1:13" s="14" customFormat="1">
+    <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13"/>
       <c r="B14" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
@@ -5147,43 +5149,43 @@
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="8:9">
+    <row r="17" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="8:9">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="8:9">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="8:9">
+    <row r="20" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="8:9">
+    <row r="21" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="8:9">
+    <row r="22" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="8:9">
+    <row r="23" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="8:9">
+    <row r="24" spans="8:9" x14ac:dyDescent="0.35">
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
@@ -5206,7 +5208,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="3"/>
@@ -5221,21 +5223,21 @@
     <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="45" customFormat="1" ht="45">
+    <row r="1" spans="1:14" s="45" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>19</v>
@@ -5247,19 +5249,19 @@
         <v>7</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K1" s="44" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
       <c r="N1" s="44"/>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="90">
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="93" x14ac:dyDescent="0.35">
       <c r="A2" s="18"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -5269,10 +5271,10 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>214</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>215</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
@@ -5280,36 +5282,36 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="45">
+    <row r="3" spans="1:14" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F3" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>142</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
     </row>
-    <row r="4" spans="1:14" s="16" customFormat="1" ht="90">
+    <row r="4" spans="1:14" s="16" customFormat="1" ht="93" x14ac:dyDescent="0.35">
       <c r="A4" s="20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -5320,7 +5322,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="1:14" s="16" customFormat="1" ht="45">
+    <row r="5" spans="1:14" s="16" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -5328,11 +5330,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20" t="b">
@@ -5342,37 +5344,37 @@
         <v>1</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="16" customFormat="1" ht="30">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="16" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F6" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>147</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>148</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" spans="1:14" s="17" customFormat="1">
+    <row r="7" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="21"/>
       <c r="B7" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -5383,31 +5385,31 @@
       <c r="J7" s="21"/>
       <c r="K7" s="21"/>
     </row>
-    <row r="8" spans="1:14" s="17" customFormat="1" ht="30">
+    <row r="8" spans="1:14" s="17" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="H8" s="21" t="s">
         <v>152</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>153</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
     </row>
-    <row r="9" spans="1:14" s="17" customFormat="1">
+    <row r="9" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="21"/>
       <c r="B9" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -5419,10 +5421,10 @@
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
     </row>
-    <row r="10" spans="1:14" s="16" customFormat="1">
+    <row r="10" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="20"/>
       <c r="B10" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
@@ -5434,34 +5436,34 @@
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:14" ht="30">
+    <row r="11" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F11" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>154</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>155</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
     </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" ht="45">
+    <row r="12" spans="1:14" s="9" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A12" s="22"/>
       <c r="B12" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -5472,7 +5474,7 @@
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" ht="45">
+    <row r="13" spans="1:14" s="9" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
@@ -5480,11 +5482,11 @@
         <v>1</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="22" t="b">
@@ -5494,13 +5496,13 @@
         <v>1</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="9" customFormat="1">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="22"/>
       <c r="B14" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -5512,34 +5514,34 @@
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
-    <row r="15" spans="1:14" ht="30">
+    <row r="15" spans="1:14" ht="31" x14ac:dyDescent="0.35">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F15" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>159</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>160</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
     </row>
-    <row r="16" spans="1:14" s="11" customFormat="1" ht="60">
+    <row r="16" spans="1:14" s="11" customFormat="1" ht="62" x14ac:dyDescent="0.35">
       <c r="A16" s="23"/>
       <c r="B16" s="23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -5550,7 +5552,7 @@
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
     </row>
-    <row r="17" spans="1:11" s="11" customFormat="1" ht="45">
+    <row r="17" spans="1:11" s="11" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -5558,11 +5560,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="23" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H17" s="23"/>
       <c r="I17" s="23" t="b">
@@ -5572,13 +5574,13 @@
         <v>1</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="11" customFormat="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="23"/>
       <c r="B18" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
@@ -5590,34 +5592,34 @@
       <c r="J18" s="23"/>
       <c r="K18" s="23"/>
     </row>
-    <row r="19" spans="1:11" ht="30">
+    <row r="19" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F19" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="G19" s="18" t="s">
         <v>164</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>165</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" spans="1:11" s="5" customFormat="1" ht="45">
+    <row r="20" spans="1:11" s="5" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A20" s="24"/>
       <c r="B20" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -5628,7 +5630,7 @@
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
     </row>
-    <row r="21" spans="1:11" s="5" customFormat="1" ht="45">
+    <row r="21" spans="1:11" s="5" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -5636,11 +5638,11 @@
         <v>1</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="24" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H21" s="24"/>
       <c r="I21" s="24" t="b">
@@ -5650,13 +5652,13 @@
         <v>1</v>
       </c>
       <c r="K21" s="24" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="5" customFormat="1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="24"/>
       <c r="B22" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
@@ -5668,34 +5670,34 @@
       <c r="J22" s="24"/>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="1:11" ht="30">
+    <row r="23" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
       <c r="D23" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F23" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="G23" s="18" t="s">
         <v>168</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>169</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" spans="1:11" s="17" customFormat="1" ht="60">
+    <row r="24" spans="1:11" s="17" customFormat="1" ht="62" x14ac:dyDescent="0.35">
       <c r="A24" s="21"/>
       <c r="B24" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -5706,7 +5708,7 @@
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:11" s="17" customFormat="1" ht="45">
+    <row r="25" spans="1:11" s="17" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -5714,11 +5716,11 @@
         <v>1</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H25" s="21"/>
       <c r="I25" s="21" t="b">
@@ -5728,13 +5730,13 @@
         <v>1</v>
       </c>
       <c r="K25" s="21" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="17" customFormat="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="21"/>
       <c r="B26" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -5746,7 +5748,7 @@
       <c r="J26" s="21"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -5756,16 +5758,16 @@
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
     </row>
-    <row r="28" spans="1:11" s="29" customFormat="1">
+    <row r="28" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="47" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>

</xml_diff>

<commit_message>
Clean up the xlsx conversion script and xlsx forms to have the correct value for true or false
</commit_message>
<xml_diff>
--- a/app/tables/Ethiopia_household/forms/Ethiopia_household_data/Ethiopia_household_data.xlsx
+++ b/app/tables/Ethiopia_household/forms/Ethiopia_household_data/Ethiopia_household_data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25540" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="30740" windowHeight="16660" tabRatio="500" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="queries" sheetId="9" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="319">
   <si>
     <t>type</t>
   </si>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t>display.hide_add_instance</t>
-  </si>
-  <si>
-    <t>TRUE</t>
   </si>
   <si>
     <t>Add House Member</t>
@@ -1295,7 +1292,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1421,6 +1418,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1929,11 +1941,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.83203125" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
@@ -1945,15 +1957,15 @@
     <col min="8" max="8" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="46" customFormat="1">
       <c r="A1" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="44" t="s">
         <v>107</v>
-      </c>
-      <c r="C1" s="44" t="s">
-        <v>108</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>3</v>
@@ -1971,9 +1983,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A2" s="36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
@@ -1983,9 +1995,9 @@
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
     </row>
-    <row r="3" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A3" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
@@ -1995,9 +2007,9 @@
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
     </row>
-    <row r="4" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A4" s="36" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
@@ -2007,9 +2019,9 @@
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
     </row>
-    <row r="5" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A5" s="36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="33"/>
@@ -2019,9 +2031,9 @@
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
     </row>
-    <row r="6" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A6" s="36" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -2031,9 +2043,9 @@
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
     </row>
-    <row r="7" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A7" s="36" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
@@ -2043,7 +2055,7 @@
       <c r="G7" s="34"/>
       <c r="H7" s="34"/>
     </row>
-    <row r="8" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="35" customFormat="1" ht="19" customHeight="1">
       <c r="A8" s="36"/>
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
@@ -2053,12 +2065,12 @@
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
     </row>
-    <row r="9" spans="1:17" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="45">
       <c r="A9" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
@@ -2076,13 +2088,13 @@
         <v>25</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="30">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>1</v>
@@ -2100,13 +2112,13 @@
         <v>25</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="30">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>1</v>
@@ -2124,15 +2136,15 @@
         <v>25</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="12" customFormat="1" ht="30" customHeight="1">
       <c r="A12" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>1</v>
@@ -2144,13 +2156,13 @@
         <v>28</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>54</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
@@ -2158,15 +2170,15 @@
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
     </row>
-    <row r="13" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B13" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>28</v>
@@ -2178,7 +2190,7 @@
         <v>25</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
@@ -2186,15 +2198,15 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
     </row>
-    <row r="14" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B14" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>28</v>
@@ -2203,10 +2215,10 @@
         <v>23</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
@@ -2214,27 +2226,27 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
     </row>
-    <row r="15" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B15" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
@@ -2242,27 +2254,27 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
     </row>
-    <row r="16" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B16" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
@@ -2270,27 +2282,27 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
     </row>
-    <row r="17" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B17" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -2298,27 +2310,27 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
     </row>
-    <row r="18" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B18" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
@@ -2326,27 +2338,27 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
     </row>
-    <row r="19" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B19" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
@@ -2354,15 +2366,15 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B20" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>28</v>
@@ -2374,7 +2386,7 @@
         <v>25</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
@@ -2382,15 +2394,15 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
     </row>
-    <row r="21" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B21" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>28</v>
@@ -2402,7 +2414,7 @@
         <v>25</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
@@ -2410,16 +2422,16 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
     </row>
-    <row r="22" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="30">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>28</v>
@@ -2428,22 +2440,22 @@
         <v>23</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="30">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>28</v>
@@ -2455,19 +2467,19 @@
         <v>25</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="30">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>28</v>
@@ -2479,19 +2491,19 @@
         <v>25</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="31" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="30">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>28</v>
@@ -2503,7 +2515,7 @@
         <v>25</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -2521,11 +2533,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38:J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="8" customWidth="1"/>
@@ -2540,21 +2552,21 @@
     <col min="11" max="11" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="45" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" s="45" customFormat="1" ht="30">
       <c r="A1" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>46</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>19</v>
@@ -2569,23 +2581,23 @@
         <v>55</v>
       </c>
       <c r="J1" s="45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K1" s="44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
       <c r="N1" s="44"/>
       <c r="O1" s="44"/>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" s="1" customFormat="1">
       <c r="A2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -2593,19 +2605,19 @@
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="90">
       <c r="A3" s="3"/>
       <c r="D3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -2613,13 +2625,13 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="10" customFormat="1" ht="30">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -2627,19 +2639,19 @@
       <c r="N4" s="9"/>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:15" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" s="10" customFormat="1" ht="30">
       <c r="A5" s="9"/>
       <c r="D5" s="10" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -2647,35 +2659,35 @@
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
     </row>
-    <row r="6" spans="1:15" s="10" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" s="10" customFormat="1" ht="75">
       <c r="A6" s="9"/>
       <c r="D6" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="I6" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>217</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>218</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" s="10" customFormat="1">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -2683,19 +2695,19 @@
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
     </row>
-    <row r="8" spans="1:15" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" s="10" customFormat="1" ht="30">
       <c r="A8" s="9"/>
       <c r="D8" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E8" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>221</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>222</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -2703,10 +2715,10 @@
       <c r="N8" s="9"/>
       <c r="O8" s="9"/>
     </row>
-    <row r="9" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" s="10" customFormat="1">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -2714,19 +2726,19 @@
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="45">
       <c r="A10" s="3"/>
       <c r="D10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -2734,13 +2746,13 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" s="12" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" s="12" customFormat="1" ht="30">
       <c r="A11" s="11"/>
       <c r="B11" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K11" s="11"/>
       <c r="L11" s="11"/>
@@ -2748,19 +2760,19 @@
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
     </row>
-    <row r="12" spans="1:15" s="12" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" s="12" customFormat="1" ht="30">
       <c r="A12" s="11"/>
       <c r="D12" s="12" t="s">
         <v>32</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F12" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>242</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>243</v>
       </c>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
@@ -2768,35 +2780,35 @@
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
     </row>
-    <row r="13" spans="1:15" s="12" customFormat="1" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" s="12" customFormat="1" ht="75">
       <c r="A13" s="11"/>
       <c r="D13" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="I13" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="11" t="s">
         <v>245</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>246</v>
       </c>
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
       <c r="N13" s="11"/>
       <c r="O13" s="11"/>
     </row>
-    <row r="14" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" s="12" customFormat="1">
       <c r="A14" s="11"/>
       <c r="B14" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
@@ -2804,7 +2816,7 @@
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
     </row>
-    <row r="15" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" s="28" customFormat="1">
       <c r="A15" s="27"/>
       <c r="K15" s="27"/>
       <c r="L15" s="27"/>
@@ -2812,13 +2824,13 @@
       <c r="N15" s="27"/>
       <c r="O15" s="27"/>
     </row>
-    <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" s="1" customFormat="1">
       <c r="A16" s="3"/>
       <c r="D16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -2826,19 +2838,19 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" s="1" customFormat="1" ht="60">
       <c r="A17" s="3"/>
       <c r="D17" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>250</v>
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -2846,13 +2858,13 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:15" s="26" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" s="26" customFormat="1" ht="30">
       <c r="A18" s="16"/>
       <c r="B18" s="26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K18" s="16"/>
       <c r="L18" s="16"/>
@@ -2860,19 +2872,19 @@
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
     </row>
-    <row r="19" spans="1:15" s="26" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" s="26" customFormat="1" ht="30">
       <c r="A19" s="16"/>
       <c r="D19" s="26" t="s">
         <v>32</v>
       </c>
       <c r="E19" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="G19" s="26" t="s">
         <v>253</v>
-      </c>
-      <c r="F19" s="26" t="s">
-        <v>252</v>
-      </c>
-      <c r="G19" s="26" t="s">
-        <v>254</v>
       </c>
       <c r="K19" s="16"/>
       <c r="L19" s="16"/>
@@ -2880,19 +2892,19 @@
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
     </row>
-    <row r="20" spans="1:15" s="26" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" s="26" customFormat="1" ht="30">
       <c r="A20" s="16"/>
       <c r="D20" s="26" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="F20" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="G20" s="26" t="s">
         <v>256</v>
-      </c>
-      <c r="G20" s="26" t="s">
-        <v>257</v>
       </c>
       <c r="K20" s="16"/>
       <c r="L20" s="16"/>
@@ -2900,13 +2912,13 @@
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
     </row>
-    <row r="21" spans="1:15" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" s="10" customFormat="1" ht="30">
       <c r="A21" s="9"/>
       <c r="B21" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
@@ -2914,19 +2926,19 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
     </row>
-    <row r="22" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" s="10" customFormat="1">
       <c r="A22" s="9"/>
       <c r="D22" s="10" t="s">
         <v>32</v>
       </c>
       <c r="E22" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>271</v>
-      </c>
       <c r="G22" s="10" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
@@ -2934,13 +2946,13 @@
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
     </row>
-    <row r="23" spans="1:15" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" s="8" customFormat="1" ht="30">
       <c r="A23" s="7"/>
       <c r="B23" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K23" s="7"/>
       <c r="L23" s="7"/>
@@ -2948,16 +2960,16 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
     </row>
-    <row r="24" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" s="8" customFormat="1">
       <c r="A24" s="7"/>
       <c r="D24" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F24" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="G24" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>282</v>
       </c>
       <c r="K24" s="7"/>
       <c r="L24" s="7"/>
@@ -2965,10 +2977,10 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
     </row>
-    <row r="25" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" s="8" customFormat="1">
       <c r="A25" s="7"/>
       <c r="B25" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
@@ -2976,10 +2988,10 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
     </row>
-    <row r="26" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" s="10" customFormat="1">
       <c r="A26" s="9"/>
       <c r="B26" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
@@ -2987,10 +2999,10 @@
       <c r="N26" s="9"/>
       <c r="O26" s="9"/>
     </row>
-    <row r="27" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" s="26" customFormat="1">
       <c r="A27" s="16"/>
       <c r="B27" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K27" s="16"/>
       <c r="L27" s="16"/>
@@ -2998,7 +3010,7 @@
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
     </row>
-    <row r="28" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" s="1" customFormat="1">
       <c r="A28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
@@ -3006,32 +3018,32 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" s="1" customFormat="1">
       <c r="A29" s="3"/>
       <c r="D29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:15" s="1" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" s="1" customFormat="1" ht="60">
       <c r="A30" s="3"/>
       <c r="D30" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
@@ -3039,13 +3051,13 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" spans="1:15" s="12" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" s="12" customFormat="1" ht="30">
       <c r="A31" s="11"/>
       <c r="B31" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
@@ -3053,28 +3065,28 @@
       <c r="N31" s="11"/>
       <c r="O31" s="11"/>
     </row>
-    <row r="32" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" s="12" customFormat="1">
       <c r="A32" s="11"/>
       <c r="D32" s="12" t="s">
         <v>1</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+      <c r="I32" s="51" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" s="51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="12" customFormat="1">
       <c r="A33" s="11"/>
       <c r="B33" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
@@ -3082,36 +3094,36 @@
       <c r="N33" s="11"/>
       <c r="O33" s="11"/>
     </row>
-    <row r="34" spans="1:15" s="30" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" s="30" customFormat="1" ht="45">
       <c r="A34" s="29" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>1</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G34" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="H34" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="H34" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="I34" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="J34" s="30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I34" s="52" t="b">
+        <v>1</v>
+      </c>
+      <c r="J34" s="52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" s="1" customFormat="1">
       <c r="A35" s="3"/>
       <c r="D35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
@@ -3119,16 +3131,16 @@
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15">
       <c r="D36" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E36" t="s">
+        <v>292</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="I36" t="b">
         <v>1</v>
       </c>
@@ -3136,23 +3148,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15">
       <c r="D37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G37" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="D38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>296</v>
-      </c>
       <c r="G38" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I38" t="b">
         <v>1</v>
@@ -3176,11 +3188,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="3" max="3" width="33.83203125" customWidth="1"/>
@@ -3191,21 +3203,21 @@
     <col min="8" max="8" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="45" customFormat="1">
       <c r="A1" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>46</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>19</v>
@@ -3222,16 +3234,16 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="105">
       <c r="A2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -3239,7 +3251,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3247,13 +3259,13 @@
         <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>31</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -3261,9 +3273,9 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="32" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" s="32" customFormat="1" ht="45">
       <c r="A4" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="31" t="s">
         <v>47</v>
@@ -3279,9 +3291,9 @@
       <c r="L4" s="31"/>
       <c r="M4" s="31"/>
     </row>
-    <row r="5" spans="1:13" s="32" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" s="32" customFormat="1" ht="30">
       <c r="A5" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
@@ -3293,7 +3305,7 @@
         <v>33</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I5" s="31"/>
       <c r="J5" s="31"/>
@@ -3301,13 +3313,13 @@
       <c r="L5" s="31"/>
       <c r="M5" s="31"/>
     </row>
-    <row r="6" spans="1:13" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" s="10" customFormat="1" ht="30">
       <c r="A6" s="9"/>
       <c r="B6" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -3319,7 +3331,7 @@
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" s="10" customFormat="1">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -3327,13 +3339,13 @@
         <v>35</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>34</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -3341,10 +3353,10 @@
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" s="10" customFormat="1">
       <c r="A8" s="9"/>
       <c r="B8" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -3357,7 +3369,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" s="32" customFormat="1">
       <c r="A9" s="31"/>
       <c r="B9" s="31" t="s">
         <v>48</v>
@@ -3373,7 +3385,7 @@
       <c r="L9" s="31"/>
       <c r="M9" s="31"/>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -3381,13 +3393,13 @@
         <v>35</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -3395,7 +3407,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" s="25" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" s="25" customFormat="1" ht="30">
       <c r="A11" s="17"/>
       <c r="B11" s="17" t="s">
         <v>47</v>
@@ -3411,7 +3423,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
     </row>
-    <row r="12" spans="1:13" s="25" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" s="25" customFormat="1" ht="30">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
@@ -3419,13 +3431,13 @@
         <v>35</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>37</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I12" s="17"/>
       <c r="J12" s="17"/>
@@ -3433,13 +3445,13 @@
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
     </row>
-    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" s="10" customFormat="1">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
@@ -3451,7 +3463,7 @@
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="1:13" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" s="10" customFormat="1" ht="30">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -3459,13 +3471,13 @@
         <v>35</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>38</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
@@ -3473,10 +3485,10 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" s="10" customFormat="1">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -3489,7 +3501,7 @@
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" s="25" customFormat="1">
       <c r="A16" s="17"/>
       <c r="B16" s="17" t="s">
         <v>48</v>
@@ -3505,7 +3517,7 @@
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
     </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -3513,13 +3525,13 @@
         <v>35</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>39</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -3527,13 +3539,13 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" s="12" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" s="12" customFormat="1" ht="30">
       <c r="A18" s="11"/>
       <c r="B18" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
@@ -3545,9 +3557,9 @@
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
     </row>
-    <row r="19" spans="1:13" s="12" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" s="12" customFormat="1" ht="30">
       <c r="A19" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -3559,7 +3571,7 @@
         <v>40</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="11"/>
@@ -3567,10 +3579,10 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" s="12" customFormat="1">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -3583,7 +3595,7 @@
       <c r="L20" s="11"/>
       <c r="M20" s="11"/>
     </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -3591,13 +3603,13 @@
         <v>35</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -3605,7 +3617,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -3613,13 +3625,13 @@
         <v>35</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>42</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -3646,7 +3658,7 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="23.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
@@ -3658,21 +3670,21 @@
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="45" customFormat="1">
       <c r="A1" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>46</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>19</v>
@@ -3689,9 +3701,9 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="45">
       <c r="A2" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>18</v>
@@ -3703,12 +3715,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" s="6" customFormat="1" ht="60">
       <c r="A5" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -3716,10 +3728,10 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" s="6" customFormat="1">
       <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -3727,10 +3739,10 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" s="6" customFormat="1">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -3738,10 +3750,10 @@
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
     </row>
-    <row r="11" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" s="6" customFormat="1">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -3749,10 +3761,10 @@
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
     </row>
-    <row r="13" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" s="6" customFormat="1">
       <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -3760,10 +3772,10 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="15" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" s="6" customFormat="1">
       <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -3771,10 +3783,10 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="17" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" s="6" customFormat="1">
       <c r="A17" s="5"/>
       <c r="B17" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -3801,275 +3813,275 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="46" customFormat="1">
       <c r="A1" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>66</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>67</v>
       </c>
       <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="37" customFormat="1">
       <c r="A2" s="37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="37" customFormat="1">
+      <c r="A3" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="37" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" s="38" customFormat="1">
       <c r="A4" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B4" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="16" t="s">
+    </row>
+    <row r="5" spans="1:3" s="38" customFormat="1">
+      <c r="A5" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="16" t="s">
+      <c r="C5" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="16" t="s">
+    </row>
+    <row r="6" spans="1:3" s="39" customFormat="1">
+      <c r="A6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="7" t="s">
+    </row>
+    <row r="7" spans="1:3" s="39" customFormat="1">
+      <c r="A7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="7" t="s">
+    </row>
+    <row r="8" spans="1:3" s="39" customFormat="1">
+      <c r="A8" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:3" s="40" customFormat="1">
       <c r="A9" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="40" customFormat="1">
+      <c r="A10" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B10" s="9" t="s">
+    <row r="11" spans="1:3" s="40" customFormat="1">
+      <c r="A11" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B11" s="9" t="s">
+    <row r="12" spans="1:3" s="40" customFormat="1">
+      <c r="A12" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B12" s="9" t="s">
+    <row r="13" spans="1:3" s="40" customFormat="1">
+      <c r="A13" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>226</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B13" s="9" t="s">
+    <row r="14" spans="1:3" s="40" customFormat="1">
+      <c r="A14" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B14" s="9" t="s">
+    <row r="15" spans="1:3" s="40" customFormat="1" ht="30">
+      <c r="A15" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C15" s="9" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="40" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A15" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" s="41" customFormat="1">
       <c r="A16" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="41" customFormat="1">
+      <c r="A17" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
-        <v>253</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="C17" s="11" t="s">
+    <row r="18" spans="1:3" s="42" customFormat="1">
+      <c r="A18" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="B18" s="13" t="s">
+      <c r="C18" s="13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="42" customFormat="1">
+      <c r="A19" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="B19" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C19" s="13" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="B19" s="13" t="s">
+    <row r="20" spans="1:3" s="42" customFormat="1">
+      <c r="A20" s="13" t="s">
+        <v>254</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C20" s="13" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" s="43" customFormat="1">
       <c r="A21" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B21" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="43" customFormat="1">
+      <c r="A22" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C22" s="17" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="17" t="s">
-        <v>270</v>
-      </c>
-      <c r="B22" s="17" t="s">
+    <row r="23" spans="1:3" s="43" customFormat="1">
+      <c r="A23" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C23" s="17" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="17" t="s">
-        <v>270</v>
-      </c>
-      <c r="B23" s="17" t="s">
+    <row r="24" spans="1:3" s="43" customFormat="1" ht="30">
+      <c r="A24" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C24" s="17" t="s">
         <v>278</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="43" customFormat="1" ht="31" x14ac:dyDescent="0.35">
-      <c r="A24" s="17" t="s">
-        <v>270</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>275</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -4091,7 +4103,7 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19" style="3" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" style="3" customWidth="1"/>
@@ -4100,7 +4112,7 @@
     <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="44" customFormat="1">
       <c r="A1" s="44" t="s">
         <v>11</v>
       </c>
@@ -4111,10 +4123,10 @@
         <v>13</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -4123,7 +4135,7 @@
       </c>
       <c r="D2" s="48"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -4132,7 +4144,7 @@
       </c>
       <c r="D3" s="48"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -4141,7 +4153,7 @@
       </c>
       <c r="D4" s="48"/>
     </row>
-    <row r="5" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -4150,72 +4162,72 @@
       </c>
       <c r="D5" s="48"/>
     </row>
-    <row r="6" spans="1:4" ht="31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="48" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="D6" s="48" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="48"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D7" s="48"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="D8" s="48"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D8" s="48"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="48"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D9" s="48"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="48"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="D10" s="48"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="48"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="D11" s="48"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="D12" s="48"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
         <v>43</v>
       </c>
@@ -4240,10 +4252,10 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="39.1640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" style="3" customWidth="1"/>
@@ -4256,15 +4268,15 @@
     <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="45" customFormat="1">
       <c r="A1" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>2</v>
@@ -4276,10 +4288,10 @@
         <v>55</v>
       </c>
       <c r="G1" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
@@ -4287,7 +4299,7 @@
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="33" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -4303,15 +4315,15 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="76" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -4320,7 +4332,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -4328,24 +4340,24 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" ht="109" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" s="1" customFormat="1" ht="109" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>56</v>
+      <c r="F4" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="49" t="b">
+        <v>1</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -4369,10 +4381,10 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
     <col min="2" max="2" width="12.5" style="3" customWidth="1"/>
@@ -4383,15 +4395,15 @@
     <col min="7" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="44" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="44" customFormat="1">
       <c r="A1" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="44" t="s">
         <v>2</v>
@@ -4400,10 +4412,10 @@
         <v>55</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -4418,29 +4430,29 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>56</v>
+      <c r="E3" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="49" t="b">
+        <v>1</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" s="1" customFormat="1">
       <c r="A4" s="3"/>
       <c r="C4" s="3"/>
       <c r="G4" s="3"/>
@@ -4464,10 +4476,10 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
@@ -4478,15 +4490,15 @@
     <col min="7" max="7" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="46" customFormat="1">
       <c r="A1" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="44" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="44" t="s">
         <v>19</v>
@@ -4498,20 +4510,20 @@
         <v>55</v>
       </c>
       <c r="G1" s="44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H1" s="44"/>
       <c r="I1" s="44"/>
       <c r="J1" s="44"/>
       <c r="K1" s="44"/>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="1" customFormat="1">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -4519,151 +4531,151 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" ht="30">
       <c r="A3" s="3"/>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>56</v>
+        <v>132</v>
+      </c>
+      <c r="F3" s="49" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="49" t="b">
+        <v>1</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="90">
       <c r="A4" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="45">
       <c r="B5" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="45">
       <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="30">
       <c r="B7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="3" customFormat="1" ht="30">
       <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="45">
       <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="45">
       <c r="B10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="3" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="3" customFormat="1" ht="30">
       <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -4676,7 +4688,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -4689,7 +4701,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -4702,7 +4714,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -4715,7 +4727,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -4728,7 +4740,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -4741,7 +4753,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4754,7 +4766,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -4767,7 +4779,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -4780,7 +4792,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -4793,7 +4805,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4806,7 +4818,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4819,7 +4831,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4832,7 +4844,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4860,11 +4872,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" style="3" customWidth="1"/>
@@ -4879,21 +4891,21 @@
     <col min="11" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="45" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="45" customFormat="1" ht="30">
       <c r="A1" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>46</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>19</v>
@@ -4905,22 +4917,22 @@
         <v>55</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K1" s="44"/>
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -4928,32 +4940,32 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A3" s="3"/>
       <c r="D3" s="3" t="s">
         <v>35</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" s="8" customFormat="1">
       <c r="A4" s="7"/>
       <c r="B4" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -4964,7 +4976,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" s="8" customFormat="1">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -4972,13 +4984,13 @@
         <v>32</v>
       </c>
       <c r="E5" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>124</v>
-      </c>
       <c r="G5" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
@@ -4987,10 +4999,10 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" s="8" customFormat="1">
       <c r="A6" s="7"/>
       <c r="B6" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -5003,19 +5015,19 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" s="8" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" s="8" customFormat="1" ht="60">
       <c r="A7" s="7"/>
       <c r="D7" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -5024,13 +5036,13 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" s="10" customFormat="1">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
@@ -5043,19 +5055,19 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" s="10" customFormat="1">
       <c r="A9" s="9"/>
       <c r="D9" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F9" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -5064,10 +5076,10 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" s="10" customFormat="1">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -5080,10 +5092,10 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" s="8" customFormat="1">
       <c r="A11" s="7"/>
       <c r="B11" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -5096,13 +5108,13 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" s="14" customFormat="1">
       <c r="A12" s="13"/>
       <c r="B12" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
@@ -5111,36 +5123,36 @@
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="1:13" s="14" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" s="14" customFormat="1" ht="90">
       <c r="A13" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>56</v>
+        <v>205</v>
+      </c>
+      <c r="H13" s="53" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="53" t="b">
+        <v>1</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
     </row>
-    <row r="14" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" s="14" customFormat="1">
       <c r="A14" s="13"/>
       <c r="B14" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
@@ -5149,43 +5161,43 @@
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13">
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13">
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="8:9">
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:9">
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="8:9">
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="8:9">
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="8:9">
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="8:9">
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="8:9">
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="8:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="8:9">
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
     </row>
@@ -5204,11 +5216,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N28"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="F15" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25:J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="3"/>
@@ -5223,21 +5235,21 @@
     <col min="12" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="45" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" s="45" customFormat="1" ht="45">
       <c r="A1" s="44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="45" t="s">
         <v>46</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="45" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>19</v>
@@ -5252,16 +5264,16 @@
         <v>55</v>
       </c>
       <c r="J1" s="44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K1" s="44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L1" s="44"/>
       <c r="M1" s="44"/>
       <c r="N1" s="44"/>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="90">
       <c r="A2" s="18"/>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -5271,10 +5283,10 @@
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>213</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>214</v>
       </c>
       <c r="I2" s="18"/>
       <c r="J2" s="18"/>
@@ -5282,7 +5294,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="45">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -5290,28 +5302,28 @@
         <v>32</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F3" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>141</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>142</v>
       </c>
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
     </row>
-    <row r="4" spans="1:14" s="16" customFormat="1" ht="93" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" s="16" customFormat="1" ht="90">
       <c r="A4" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -5322,7 +5334,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
     </row>
-    <row r="5" spans="1:14" s="16" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" s="16" customFormat="1" ht="45">
       <c r="A5" s="20"/>
       <c r="B5" s="20"/>
       <c r="C5" s="20"/>
@@ -5330,11 +5342,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20" t="b">
@@ -5344,10 +5356,10 @@
         <v>1</v>
       </c>
       <c r="K5" s="20" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="16" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="16" customFormat="1" ht="30">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -5355,26 +5367,26 @@
         <v>35</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>146</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>147</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
     </row>
-    <row r="7" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" s="17" customFormat="1">
       <c r="A7" s="21"/>
       <c r="B7" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
@@ -5385,31 +5397,31 @@
       <c r="J7" s="21"/>
       <c r="K7" s="21"/>
     </row>
-    <row r="8" spans="1:14" s="17" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" s="17" customFormat="1" ht="30">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="H8" s="21" t="s">
         <v>151</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>152</v>
       </c>
       <c r="I8" s="21"/>
       <c r="J8" s="21"/>
       <c r="K8" s="21"/>
     </row>
-    <row r="9" spans="1:14" s="17" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" s="17" customFormat="1">
       <c r="A9" s="21"/>
       <c r="B9" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
@@ -5421,10 +5433,10 @@
       <c r="J9" s="21"/>
       <c r="K9" s="21"/>
     </row>
-    <row r="10" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" s="16" customFormat="1">
       <c r="A10" s="20"/>
       <c r="B10" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
@@ -5436,7 +5448,7 @@
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:14" ht="31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" ht="30">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -5444,26 +5456,26 @@
         <v>32</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F11" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="G11" s="18" t="s">
         <v>153</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>154</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
     </row>
-    <row r="12" spans="1:14" s="9" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" s="9" customFormat="1" ht="45">
       <c r="A12" s="22"/>
       <c r="B12" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D12" s="22"/>
       <c r="E12" s="22"/>
@@ -5474,7 +5486,7 @@
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" s="9" customFormat="1" ht="45">
       <c r="A13" s="22"/>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
@@ -5482,11 +5494,11 @@
         <v>1</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="22" t="b">
@@ -5496,13 +5508,13 @@
         <v>1</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="9" customFormat="1">
       <c r="A14" s="22"/>
       <c r="B14" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
@@ -5514,7 +5526,7 @@
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
-    <row r="15" spans="1:14" ht="31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" ht="30">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -5522,26 +5534,26 @@
         <v>32</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F15" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="G15" s="18" t="s">
         <v>158</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>159</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
       <c r="J15" s="18"/>
       <c r="K15" s="18"/>
     </row>
-    <row r="16" spans="1:14" s="11" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" s="11" customFormat="1" ht="60">
       <c r="A16" s="23"/>
       <c r="B16" s="23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -5552,7 +5564,7 @@
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
     </row>
-    <row r="17" spans="1:11" s="11" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" s="11" customFormat="1" ht="45">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -5560,11 +5572,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H17" s="23"/>
       <c r="I17" s="23" t="b">
@@ -5574,13 +5586,13 @@
         <v>1</v>
       </c>
       <c r="K17" s="23" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="11" customFormat="1" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="11" customFormat="1">
       <c r="A18" s="23"/>
       <c r="B18" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
@@ -5592,7 +5604,7 @@
       <c r="J18" s="23"/>
       <c r="K18" s="23"/>
     </row>
-    <row r="19" spans="1:11" ht="31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="30">
       <c r="A19" s="18"/>
       <c r="B19" s="18"/>
       <c r="C19" s="18"/>
@@ -5600,26 +5612,26 @@
         <v>32</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F19" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="G19" s="18" t="s">
         <v>163</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>164</v>
       </c>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18"/>
     </row>
-    <row r="20" spans="1:11" s="5" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" s="5" customFormat="1" ht="45">
       <c r="A20" s="24"/>
       <c r="B20" s="24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
@@ -5630,7 +5642,7 @@
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
     </row>
-    <row r="21" spans="1:11" s="5" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" s="5" customFormat="1" ht="45">
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
       <c r="C21" s="24"/>
@@ -5638,11 +5650,11 @@
         <v>1</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F21" s="24"/>
       <c r="G21" s="24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H21" s="24"/>
       <c r="I21" s="24" t="b">
@@ -5652,13 +5664,13 @@
         <v>1</v>
       </c>
       <c r="K21" s="24" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.35">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="5" customFormat="1">
       <c r="A22" s="24"/>
       <c r="B22" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
@@ -5670,7 +5682,7 @@
       <c r="J22" s="24"/>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="1:11" ht="31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="30">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -5678,26 +5690,26 @@
         <v>32</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F23" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G23" s="18" t="s">
         <v>167</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>168</v>
       </c>
       <c r="H23" s="18"/>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18"/>
     </row>
-    <row r="24" spans="1:11" s="17" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" s="17" customFormat="1" ht="60">
       <c r="A24" s="21"/>
       <c r="B24" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -5708,7 +5720,7 @@
       <c r="J24" s="21"/>
       <c r="K24" s="21"/>
     </row>
-    <row r="25" spans="1:11" s="17" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" s="17" customFormat="1" ht="45">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
@@ -5716,11 +5728,11 @@
         <v>1</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F25" s="21"/>
       <c r="G25" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H25" s="21"/>
       <c r="I25" s="21" t="b">
@@ -5730,13 +5742,13 @@
         <v>1</v>
       </c>
       <c r="K25" s="21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.35">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="17" customFormat="1">
       <c r="A26" s="21"/>
       <c r="B26" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -5748,7 +5760,7 @@
       <c r="J26" s="21"/>
       <c r="K26" s="21"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -5758,16 +5770,16 @@
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18"/>
     </row>
-    <row r="28" spans="1:11" s="29" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" s="29" customFormat="1">
       <c r="A28" s="47" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B28" s="47"/>
       <c r="C28" s="47"/>

</xml_diff>